<commit_message>
fix: mitigate API throttling by increasing fetch sleep range
</commit_message>
<xml_diff>
--- a/sandbox/data_required_list.xlsx
+++ b/sandbox/data_required_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev_Environment\equity-fundamental-engine\sandbox\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9387CC6-6A7B-4D07-975F-BFC872217489}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01B52F80-B042-4A06-AABA-F3A8B190A57E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D11BE8E1-C99B-4A1A-9707-ECBA7183B913}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{D11BE8E1-C99B-4A1A-9707-ECBA7183B913}"/>
   </bookViews>
   <sheets>
     <sheet name="stock.get_info()" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="stock.get_cash_flow()" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'stock.get_balance_sheet()'!$A$1:$C$88</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'stock.get_balance_sheet()'!$A$1:$C$90</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'stock.get_cash_flow()'!$A$1:$C$60</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'stock.get_income_stmt()'!$A$1:$C$52</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'stock.get_info()'!$A$1:$E$166</definedName>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="407">
   <si>
     <t>S.No</t>
   </si>
@@ -1263,6 +1263,9 @@
   </si>
   <si>
     <t>Dynamic</t>
+  </si>
+  <si>
+    <t>PreferredStockEquity</t>
   </si>
 </sst>
 </file>
@@ -1299,7 +1302,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -1322,24 +1325,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1375,12 +1365,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1393,6 +1377,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1729,7 +1714,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{240C12F6-F3FB-4A3C-8624-8457F87BC2D7}">
   <dimension ref="A1:E166"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
@@ -1755,7 +1740,7 @@
       <c r="D1" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="18" t="s">
         <v>403</v>
       </c>
     </row>
@@ -4572,29 +4557,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDCFF331-AF48-4D4B-8BA6-136D7307FA07}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:C88"/>
+  <dimension ref="A1:C90"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="16"/>
-    <col min="2" max="2" width="55" style="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.5546875" style="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="8.88671875" style="17"/>
+    <col min="1" max="1" width="8.88671875" style="14"/>
+    <col min="2" max="2" width="55" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.88671875" style="15"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="13" t="s">
         <v>203</v>
       </c>
     </row>
@@ -4602,18 +4586,18 @@
       <c r="A2" s="12">
         <v>1</v>
       </c>
-      <c r="B2" s="14" t="s">
+      <c r="B2" s="10" t="s">
         <v>207</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="3" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="12">
         <v>2</v>
       </c>
-      <c r="B3" s="14" t="s">
+      <c r="B3" s="10" t="s">
         <v>208</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -4624,7 +4608,7 @@
       <c r="A4" s="12">
         <v>3</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="10" t="s">
         <v>209</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -4635,7 +4619,7 @@
       <c r="A5" s="12">
         <v>4</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="10" t="s">
         <v>210</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -4646,7 +4630,7 @@
       <c r="A6" s="12">
         <v>5</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="B6" s="10" t="s">
         <v>216</v>
       </c>
       <c r="C6" s="3" t="s">
@@ -4657,7 +4641,7 @@
       <c r="A7" s="12">
         <v>6</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="10" t="s">
         <v>217</v>
       </c>
       <c r="C7" s="3" t="s">
@@ -4668,7 +4652,7 @@
       <c r="A8" s="12">
         <v>7</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="10" t="s">
         <v>218</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -4679,7 +4663,7 @@
       <c r="A9" s="12">
         <v>8</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="10" t="s">
         <v>219</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -4690,7 +4674,7 @@
       <c r="A10" s="12">
         <v>9</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="10" t="s">
         <v>220</v>
       </c>
       <c r="C10" s="3" t="s">
@@ -4701,7 +4685,7 @@
       <c r="A11" s="12">
         <v>10</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="10" t="s">
         <v>221</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -4712,7 +4696,7 @@
       <c r="A12" s="12">
         <v>11</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="10" t="s">
         <v>222</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -4723,7 +4707,7 @@
       <c r="A13" s="12">
         <v>12</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="10" t="s">
         <v>223</v>
       </c>
       <c r="C13" s="3" t="s">
@@ -4734,7 +4718,7 @@
       <c r="A14" s="12">
         <v>13</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="10" t="s">
         <v>224</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -4745,7 +4729,7 @@
       <c r="A15" s="12">
         <v>14</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="10" t="s">
         <v>225</v>
       </c>
       <c r="C15" s="3" t="s">
@@ -4756,7 +4740,7 @@
       <c r="A16" s="12">
         <v>15</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="10" t="s">
         <v>226</v>
       </c>
       <c r="C16" s="3" t="s">
@@ -4767,40 +4751,40 @@
       <c r="A17" s="12">
         <v>16</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="10" t="s">
         <v>227</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="18" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18" s="12">
         <v>17</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="10" t="s">
         <v>228</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="19" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>18</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="10" t="s">
         <v>229</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="20" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>19</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="10" t="s">
         <v>230</v>
       </c>
       <c r="C20" s="3" t="s">
@@ -4811,7 +4795,7 @@
       <c r="A21" s="12">
         <v>20</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="10" t="s">
         <v>231</v>
       </c>
       <c r="C21" s="3" t="s">
@@ -4822,7 +4806,7 @@
       <c r="A22" s="12">
         <v>21</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="10" t="s">
         <v>232</v>
       </c>
       <c r="C22" s="3" t="s">
@@ -4833,29 +4817,29 @@
       <c r="A23" s="12">
         <v>22</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="10" t="s">
         <v>233</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="24" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
         <v>23</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="10" t="s">
         <v>234</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="25" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="12">
         <v>24</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="10" t="s">
         <v>235</v>
       </c>
       <c r="C25" s="3" t="s">
@@ -4866,18 +4850,18 @@
       <c r="A26" s="12">
         <v>25</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="10" t="s">
         <v>236</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="27" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
         <v>26</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="10" t="s">
         <v>237</v>
       </c>
       <c r="C27" s="3" t="s">
@@ -4888,18 +4872,18 @@
       <c r="A28" s="12">
         <v>27</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="10" t="s">
         <v>238</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="29" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
         <v>28</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="10" t="s">
         <v>239</v>
       </c>
       <c r="C29" s="3" t="s">
@@ -4910,7 +4894,7 @@
       <c r="A30" s="12">
         <v>29</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="10" t="s">
         <v>240</v>
       </c>
       <c r="C30" s="3" t="s">
@@ -4921,7 +4905,7 @@
       <c r="A31" s="12">
         <v>30</v>
       </c>
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="10" t="s">
         <v>241</v>
       </c>
       <c r="C31" s="3" t="s">
@@ -4932,73 +4916,73 @@
       <c r="A32" s="12">
         <v>31</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="10" t="s">
         <v>242</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="33" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
         <v>32</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="10" t="s">
         <v>243</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="34" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="12">
         <v>33</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="10" t="s">
         <v>244</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="12">
         <v>34</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="10" t="s">
         <v>245</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="36" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="12">
         <v>35</v>
       </c>
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="10" t="s">
         <v>246</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="37" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="12">
         <v>36</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="10" t="s">
         <v>247</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="38" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="12">
         <v>37</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="B38" s="10" t="s">
         <v>248</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -5009,7 +4993,7 @@
       <c r="A39" s="12">
         <v>38</v>
       </c>
-      <c r="B39" s="14" t="s">
+      <c r="B39" s="10" t="s">
         <v>249</v>
       </c>
       <c r="C39" s="3" t="s">
@@ -5020,7 +5004,7 @@
       <c r="A40" s="12">
         <v>39</v>
       </c>
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="10" t="s">
         <v>250</v>
       </c>
       <c r="C40" s="3" t="s">
@@ -5031,106 +5015,106 @@
       <c r="A41" s="12">
         <v>40</v>
       </c>
-      <c r="B41" s="14" t="s">
+      <c r="B41" s="10" t="s">
         <v>251</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="42" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="12">
         <v>41</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="B42" s="10" t="s">
         <v>252</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="43" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="12">
         <v>42</v>
       </c>
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="10" t="s">
         <v>253</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="44" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="12">
         <v>43</v>
       </c>
-      <c r="B44" s="14" t="s">
+      <c r="B44" s="10" t="s">
         <v>254</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="45" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="12">
         <v>44</v>
       </c>
-      <c r="B45" s="14" t="s">
+      <c r="B45" s="10" t="s">
         <v>255</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="46" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="12">
         <v>45</v>
       </c>
-      <c r="B46" s="14" t="s">
+      <c r="B46" s="10" t="s">
         <v>256</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="47" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="12">
         <v>46</v>
       </c>
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="10" t="s">
         <v>257</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="48" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="12">
         <v>47</v>
       </c>
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="10" t="s">
         <v>258</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="49" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="12">
         <v>48</v>
       </c>
-      <c r="B49" s="14" t="s">
+      <c r="B49" s="10" t="s">
         <v>259</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="50" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="12">
         <v>49</v>
       </c>
-      <c r="B50" s="14" t="s">
+      <c r="B50" s="10" t="s">
         <v>260</v>
       </c>
       <c r="C50" s="3" t="s">
@@ -5141,18 +5125,18 @@
       <c r="A51" s="12">
         <v>50</v>
       </c>
-      <c r="B51" s="14" t="s">
+      <c r="B51" s="10" t="s">
         <v>261</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="52" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A52" s="12">
         <v>51</v>
       </c>
-      <c r="B52" s="14" t="s">
+      <c r="B52" s="10" t="s">
         <v>262</v>
       </c>
       <c r="C52" s="3" t="s">
@@ -5163,7 +5147,7 @@
       <c r="A53" s="12">
         <v>52</v>
       </c>
-      <c r="B53" s="14" t="s">
+      <c r="B53" s="10" t="s">
         <v>263</v>
       </c>
       <c r="C53" s="3" t="s">
@@ -5174,95 +5158,95 @@
       <c r="A54" s="12">
         <v>53</v>
       </c>
-      <c r="B54" s="14" t="s">
+      <c r="B54" s="10" t="s">
         <v>264</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="55" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A55" s="12">
         <v>54</v>
       </c>
-      <c r="B55" s="14" t="s">
+      <c r="B55" s="10" t="s">
         <v>265</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="56" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A56" s="12">
         <v>55</v>
       </c>
-      <c r="B56" s="14" t="s">
+      <c r="B56" s="10" t="s">
         <v>266</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A57" s="12">
         <v>56</v>
       </c>
-      <c r="B57" s="14" t="s">
+      <c r="B57" s="10" t="s">
         <v>267</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="58" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A58" s="12">
         <v>57</v>
       </c>
-      <c r="B58" s="14" t="s">
+      <c r="B58" s="10" t="s">
         <v>268</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="59" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A59" s="12">
         <v>58</v>
       </c>
-      <c r="B59" s="14" t="s">
+      <c r="B59" s="10" t="s">
         <v>269</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="60" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A60" s="12">
         <v>59</v>
       </c>
-      <c r="B60" s="14" t="s">
+      <c r="B60" s="10" t="s">
         <v>270</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="61" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A61" s="12">
         <v>60</v>
       </c>
-      <c r="B61" s="14" t="s">
+      <c r="B61" s="10" t="s">
         <v>271</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="62" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62" s="12">
         <v>61</v>
       </c>
-      <c r="B62" s="14" t="s">
+      <c r="B62" s="10" t="s">
         <v>272</v>
       </c>
       <c r="C62" s="3" t="s">
@@ -5273,7 +5257,7 @@
       <c r="A63" s="12">
         <v>62</v>
       </c>
-      <c r="B63" s="14" t="s">
+      <c r="B63" s="10" t="s">
         <v>273</v>
       </c>
       <c r="C63" s="3" t="s">
@@ -5284,7 +5268,7 @@
       <c r="A64" s="12">
         <v>63</v>
       </c>
-      <c r="B64" s="14" t="s">
+      <c r="B64" s="10" t="s">
         <v>274</v>
       </c>
       <c r="C64" s="3" t="s">
@@ -5295,7 +5279,7 @@
       <c r="A65" s="12">
         <v>64</v>
       </c>
-      <c r="B65" s="14" t="s">
+      <c r="B65" s="10" t="s">
         <v>275</v>
       </c>
       <c r="C65" s="3" t="s">
@@ -5306,7 +5290,7 @@
       <c r="A66" s="12">
         <v>65</v>
       </c>
-      <c r="B66" s="14" t="s">
+      <c r="B66" s="10" t="s">
         <v>276</v>
       </c>
       <c r="C66" s="3" t="s">
@@ -5317,40 +5301,40 @@
       <c r="A67" s="12">
         <v>66</v>
       </c>
-      <c r="B67" s="14" t="s">
+      <c r="B67" s="10" t="s">
         <v>277</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="68" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A68" s="12">
         <v>67</v>
       </c>
-      <c r="B68" s="14" t="s">
+      <c r="B68" s="10" t="s">
         <v>278</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="69" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A69" s="12">
         <v>68</v>
       </c>
-      <c r="B69" s="14" t="s">
+      <c r="B69" s="10" t="s">
         <v>279</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="70" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A70" s="12">
         <v>69</v>
       </c>
-      <c r="B70" s="14" t="s">
+      <c r="B70" s="10" t="s">
         <v>280</v>
       </c>
       <c r="C70" s="3" t="s">
@@ -5361,7 +5345,7 @@
       <c r="A71" s="12">
         <v>70</v>
       </c>
-      <c r="B71" s="14" t="s">
+      <c r="B71" s="10" t="s">
         <v>281</v>
       </c>
       <c r="C71" s="3" t="s">
@@ -5372,18 +5356,18 @@
       <c r="A72" s="12">
         <v>71</v>
       </c>
-      <c r="B72" s="14" t="s">
+      <c r="B72" s="10" t="s">
         <v>211</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="73" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A73" s="12">
         <v>72</v>
       </c>
-      <c r="B73" s="14" t="s">
+      <c r="B73" s="10" t="s">
         <v>212</v>
       </c>
       <c r="C73" s="3" t="s">
@@ -5394,7 +5378,7 @@
       <c r="A74" s="12">
         <v>73</v>
       </c>
-      <c r="B74" s="14" t="s">
+      <c r="B74" s="10" t="s">
         <v>213</v>
       </c>
       <c r="C74" s="3" t="s">
@@ -5405,51 +5389,51 @@
       <c r="A75" s="12">
         <v>74</v>
       </c>
-      <c r="B75" s="14" t="s">
+      <c r="B75" s="10" t="s">
         <v>214</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="76" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A76" s="12">
         <v>75</v>
       </c>
-      <c r="B76" s="14" t="s">
+      <c r="B76" s="10" t="s">
         <v>215</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="77" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A77" s="12">
         <v>76</v>
       </c>
-      <c r="B77" s="14" t="s">
+      <c r="B77" s="10" t="s">
         <v>206</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="78" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A78" s="12">
         <v>77</v>
       </c>
-      <c r="B78" s="14" t="s">
+      <c r="B78" s="10" t="s">
         <v>282</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A79" s="12">
         <v>78</v>
       </c>
-      <c r="B79" s="14" t="s">
+      <c r="B79" s="10" t="s">
         <v>283</v>
       </c>
       <c r="C79" s="3" t="s">
@@ -5460,7 +5444,7 @@
       <c r="A80" s="12">
         <v>79</v>
       </c>
-      <c r="B80" s="14" t="s">
+      <c r="B80" s="10" t="s">
         <v>284</v>
       </c>
       <c r="C80" s="3" t="s">
@@ -5471,62 +5455,62 @@
       <c r="A81" s="12">
         <v>80</v>
       </c>
-      <c r="B81" s="14" t="s">
+      <c r="B81" s="10" t="s">
         <v>285</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="82" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A82" s="12">
         <v>81</v>
       </c>
-      <c r="B82" s="14" t="s">
+      <c r="B82" s="10" t="s">
         <v>286</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="83" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A83" s="12">
         <v>82</v>
       </c>
-      <c r="B83" s="14" t="s">
+      <c r="B83" s="10" t="s">
         <v>287</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="84" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A84" s="12">
         <v>83</v>
       </c>
-      <c r="B84" s="14" t="s">
+      <c r="B84" s="10" t="s">
         <v>288</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="85" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="12">
         <v>84</v>
       </c>
-      <c r="B85" s="14" t="s">
+      <c r="B85" s="10" t="s">
         <v>289</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="86" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86" s="12">
         <v>85</v>
       </c>
-      <c r="B86" s="14" t="s">
+      <c r="B86" s="10" t="s">
         <v>290</v>
       </c>
       <c r="C86" s="3" t="s">
@@ -5537,14 +5521,14 @@
       <c r="A87" s="12">
         <v>86</v>
       </c>
-      <c r="B87" s="14" t="s">
+      <c r="B87" s="10" t="s">
         <v>291</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="88" spans="1:3" customFormat="1" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:3" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88" s="12">
         <v>87</v>
       </c>
@@ -5555,31 +5539,46 @@
         <v>204</v>
       </c>
     </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A89" s="12">
+        <v>88</v>
+      </c>
+      <c r="B89" s="12" t="s">
+        <v>406</v>
+      </c>
+      <c r="C89" s="19" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A90" s="12">
+        <v>89</v>
+      </c>
+      <c r="B90" s="12" t="s">
+        <v>265</v>
+      </c>
+      <c r="C90" s="19" t="s">
+        <v>205</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C88" xr:uid="{FDCFF331-AF48-4D4B-8BA6-136D7307FA07}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Yes"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:C90" xr:uid="{FDCFF331-AF48-4D4B-8BA6-136D7307FA07}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88884BF3-783F-4519-9F6E-56B13CDCF165}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:C52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+      <selection activeCell="I47" sqref="I47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="11"/>
-    <col min="2" max="2" width="50.109375" style="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.109375" style="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -5594,7 +5593,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="19">
+      <c r="A2" s="17">
         <v>1</v>
       </c>
       <c r="B2" s="10" t="s">
@@ -5605,7 +5604,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="19">
+      <c r="A3" s="17">
         <v>2</v>
       </c>
       <c r="B3" s="10" t="s">
@@ -5616,7 +5615,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="19">
+      <c r="A4" s="17">
         <v>3</v>
       </c>
       <c r="B4" s="10" t="s">
@@ -5627,7 +5626,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="19">
+      <c r="A5" s="17">
         <v>4</v>
       </c>
       <c r="B5" s="10" t="s">
@@ -5637,8 +5636,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="6" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="19">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="17">
         <v>5</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -5649,7 +5648,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="19">
+      <c r="A7" s="17">
         <v>6</v>
       </c>
       <c r="B7" s="10" t="s">
@@ -5659,8 +5658,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="8" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="19">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="17">
         <v>7</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -5671,7 +5670,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="19">
+      <c r="A9" s="17">
         <v>8</v>
       </c>
       <c r="B9" s="10" t="s">
@@ -5682,7 +5681,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="19">
+      <c r="A10" s="17">
         <v>9</v>
       </c>
       <c r="B10" s="10" t="s">
@@ -5693,7 +5692,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="19">
+      <c r="A11" s="17">
         <v>10</v>
       </c>
       <c r="B11" s="10" t="s">
@@ -5703,8 +5702,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="12" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="19">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="17">
         <v>11</v>
       </c>
       <c r="B12" s="10" t="s">
@@ -5715,7 +5714,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="19">
+      <c r="A13" s="17">
         <v>12</v>
       </c>
       <c r="B13" s="10" t="s">
@@ -5726,7 +5725,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="19">
+      <c r="A14" s="17">
         <v>13</v>
       </c>
       <c r="B14" s="10" t="s">
@@ -5736,8 +5735,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="15" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="19">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="17">
         <v>14</v>
       </c>
       <c r="B15" s="10" t="s">
@@ -5747,8 +5746,8 @@
         <v>204</v>
       </c>
     </row>
-    <row r="16" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="19">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="17">
         <v>15</v>
       </c>
       <c r="B16" s="10" t="s">
@@ -5759,7 +5758,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="19">
+      <c r="A17" s="17">
         <v>16</v>
       </c>
       <c r="B17" s="10" t="s">
@@ -5770,7 +5769,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="19">
+      <c r="A18" s="17">
         <v>17</v>
       </c>
       <c r="B18" s="10" t="s">
@@ -5781,7 +5780,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A19" s="19">
+      <c r="A19" s="17">
         <v>18</v>
       </c>
       <c r="B19" s="10" t="s">
@@ -5792,7 +5791,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A20" s="19">
+      <c r="A20" s="17">
         <v>19</v>
       </c>
       <c r="B20" s="10" t="s">
@@ -5803,7 +5802,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="19">
+      <c r="A21" s="17">
         <v>20</v>
       </c>
       <c r="B21" s="10" t="s">
@@ -5813,8 +5812,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="22" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="19">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="17">
         <v>21</v>
       </c>
       <c r="B22" s="10" t="s">
@@ -5825,7 +5824,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="19">
+      <c r="A23" s="17">
         <v>22</v>
       </c>
       <c r="B23" s="10" t="s">
@@ -5835,8 +5834,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="24" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="19">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="17">
         <v>23</v>
       </c>
       <c r="B24" s="10" t="s">
@@ -5847,7 +5846,7 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="19">
+      <c r="A25" s="17">
         <v>24</v>
       </c>
       <c r="B25" s="10" t="s">
@@ -5858,7 +5857,7 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="19">
+      <c r="A26" s="17">
         <v>25</v>
       </c>
       <c r="B26" s="10" t="s">
@@ -5868,8 +5867,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="27" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="19">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" s="17">
         <v>26</v>
       </c>
       <c r="B27" s="10" t="s">
@@ -5879,8 +5878,8 @@
         <v>204</v>
       </c>
     </row>
-    <row r="28" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="19">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" s="17">
         <v>27</v>
       </c>
       <c r="B28" s="10" t="s">
@@ -5890,8 +5889,8 @@
         <v>204</v>
       </c>
     </row>
-    <row r="29" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="19">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" s="17">
         <v>28</v>
       </c>
       <c r="B29" s="10" t="s">
@@ -5902,7 +5901,7 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="19">
+      <c r="A30" s="17">
         <v>29</v>
       </c>
       <c r="B30" s="10" t="s">
@@ -5913,7 +5912,7 @@
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="19">
+      <c r="A31" s="17">
         <v>30</v>
       </c>
       <c r="B31" s="10" t="s">
@@ -5924,7 +5923,7 @@
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="19">
+      <c r="A32" s="17">
         <v>31</v>
       </c>
       <c r="B32" s="10" t="s">
@@ -5934,8 +5933,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="33" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="19">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" s="17">
         <v>32</v>
       </c>
       <c r="B33" s="10" t="s">
@@ -5945,8 +5944,8 @@
         <v>204</v>
       </c>
     </row>
-    <row r="34" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="19">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A34" s="17">
         <v>33</v>
       </c>
       <c r="B34" s="10" t="s">
@@ -5956,8 +5955,8 @@
         <v>204</v>
       </c>
     </row>
-    <row r="35" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="19">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" s="17">
         <v>34</v>
       </c>
       <c r="B35" s="10" t="s">
@@ -5968,7 +5967,7 @@
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A36" s="19">
+      <c r="A36" s="17">
         <v>35</v>
       </c>
       <c r="B36" s="10" t="s">
@@ -5978,8 +5977,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="37" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="19">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" s="17">
         <v>36</v>
       </c>
       <c r="B37" s="10" t="s">
@@ -5989,8 +5988,8 @@
         <v>204</v>
       </c>
     </row>
-    <row r="38" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="19">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" s="17">
         <v>37</v>
       </c>
       <c r="B38" s="10" t="s">
@@ -6000,8 +5999,8 @@
         <v>204</v>
       </c>
     </row>
-    <row r="39" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="19">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A39" s="17">
         <v>38</v>
       </c>
       <c r="B39" s="10" t="s">
@@ -6012,7 +6011,7 @@
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="19">
+      <c r="A40" s="17">
         <v>39</v>
       </c>
       <c r="B40" s="10" t="s">
@@ -6023,7 +6022,7 @@
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="19">
+      <c r="A41" s="17">
         <v>40</v>
       </c>
       <c r="B41" s="10" t="s">
@@ -6033,8 +6032,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="42" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="19">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" s="17">
         <v>41</v>
       </c>
       <c r="B42" s="10" t="s">
@@ -6045,7 +6044,7 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="19">
+      <c r="A43" s="17">
         <v>42</v>
       </c>
       <c r="B43" s="10" t="s">
@@ -6056,7 +6055,7 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A44" s="19">
+      <c r="A44" s="17">
         <v>43</v>
       </c>
       <c r="B44" s="10" t="s">
@@ -6067,7 +6066,7 @@
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A45" s="19">
+      <c r="A45" s="17">
         <v>44</v>
       </c>
       <c r="B45" s="10" t="s">
@@ -6078,7 +6077,7 @@
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A46" s="19">
+      <c r="A46" s="17">
         <v>45</v>
       </c>
       <c r="B46" s="10" t="s">
@@ -6089,7 +6088,7 @@
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A47" s="19">
+      <c r="A47" s="17">
         <v>46</v>
       </c>
       <c r="B47" s="10" t="s">
@@ -6100,7 +6099,7 @@
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A48" s="19">
+      <c r="A48" s="17">
         <v>47</v>
       </c>
       <c r="B48" s="10" t="s">
@@ -6111,7 +6110,7 @@
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="19">
+      <c r="A49" s="17">
         <v>48</v>
       </c>
       <c r="B49" s="10" t="s">
@@ -6122,7 +6121,7 @@
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A50" s="19">
+      <c r="A50" s="17">
         <v>49</v>
       </c>
       <c r="B50" s="10" t="s">
@@ -6132,8 +6131,8 @@
         <v>205</v>
       </c>
     </row>
-    <row r="51" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="19">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A51" s="17">
         <v>50</v>
       </c>
       <c r="B51" s="10" t="s">
@@ -6143,8 +6142,8 @@
         <v>204</v>
       </c>
     </row>
-    <row r="52" spans="1:3" hidden="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="19">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" s="17">
         <v>51</v>
       </c>
       <c r="B52" s="10" t="s">
@@ -6155,13 +6154,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C52" xr:uid="{88884BF3-783F-4519-9F6E-56B13CDCF165}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Yes"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:C52" xr:uid="{88884BF3-783F-4519-9F6E-56B13CDCF165}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>